<commit_message>
fix order of level in potential outcomes in tot-tut table
</commit_message>
<xml_diff>
--- a/Tables/tot_tut.xlsx
+++ b/Tables/tot_tut.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaac\Dropbox\Apps\Overleaf\Donde2022\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D7D841-58E9-4869-9423-E77E36CB1E0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10D0398B-1EE2-4DB6-A471-D152804EF24D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20475" yWindow="-13980" windowWidth="21600" windowHeight="11235" xr2:uid="{1119F9E7-C0AD-4EB5-B95A-549D4A6138CF}"/>
+    <workbookView xWindow="10" yWindow="10" windowWidth="19180" windowHeight="11260" xr2:uid="{1119F9E7-C0AD-4EB5-B95A-549D4A6138CF}"/>
   </bookViews>
   <sheets>
     <sheet name="tot_tut" sheetId="1" r:id="rId1"/>
@@ -302,16 +302,16 @@
         </row>
         <row r="14">
           <cell r="B14" t="str">
-            <v>-56.8***</v>
+            <v>-47.4***</v>
           </cell>
           <cell r="C14" t="str">
-            <v>-942.4***</v>
+            <v>-759.4***</v>
           </cell>
           <cell r="D14" t="str">
-            <v>56.4***</v>
+            <v>64.2***</v>
           </cell>
           <cell r="E14" t="str">
-            <v>60.9***</v>
+            <v>67.2***</v>
           </cell>
         </row>
         <row r="15">
@@ -333,16 +333,16 @@
         </row>
         <row r="17">
           <cell r="B17" t="str">
-            <v>-47.4***</v>
+            <v>-56.8***</v>
           </cell>
           <cell r="C17" t="str">
-            <v>-759.4***</v>
+            <v>-942.4***</v>
           </cell>
           <cell r="D17" t="str">
-            <v>64.2***</v>
+            <v>56.4***</v>
           </cell>
           <cell r="E17" t="str">
-            <v>67.2***</v>
+            <v>60.9***</v>
           </cell>
         </row>
         <row r="18">
@@ -833,7 +833,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{254A23C4-4F24-410C-AB8B-7C80ABB413D1}">
   <dimension ref="A2:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
       <selection activeCell="E25" sqref="A2:E25"/>
     </sheetView>
   </sheetViews>
@@ -1021,19 +1021,19 @@
       </c>
       <c r="B10" s="6" t="str">
         <f>[1]tot_tut!B14</f>
-        <v>-56.8***</v>
+        <v>-47.4***</v>
       </c>
       <c r="C10" s="6" t="str">
         <f>[1]tot_tut!C14</f>
-        <v>-942.4***</v>
+        <v>-759.4***</v>
       </c>
       <c r="D10" s="6" t="str">
         <f>[1]tot_tut!D14</f>
-        <v>56.4***</v>
+        <v>64.2***</v>
       </c>
       <c r="E10" s="6" t="str">
         <f>[1]tot_tut!E14</f>
-        <v>60.9***</v>
+        <v>67.2***</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -1064,19 +1064,19 @@
       </c>
       <c r="B12" s="6" t="str">
         <f>[1]tot_tut!B17</f>
-        <v>-47.4***</v>
+        <v>-56.8***</v>
       </c>
       <c r="C12" s="6" t="str">
         <f>[1]tot_tut!C17</f>
-        <v>-759.4***</v>
+        <v>-942.4***</v>
       </c>
       <c r="D12" s="6" t="str">
         <f>[1]tot_tut!D17</f>
-        <v>64.2***</v>
+        <v>56.4***</v>
       </c>
       <c r="E12" s="6" t="str">
         <f>[1]tot_tut!E17</f>
-        <v>67.2***</v>
+        <v>60.9***</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>